<commit_message>
final module java web
</commit_message>
<xml_diff>
--- a/Learning Detail.xlsx
+++ b/Learning Detail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
   <si>
     <t>mon</t>
   </si>
@@ -111,6 +111,71 @@
   </si>
   <si>
     <t>learn korea character</t>
+  </si>
+  <si>
+    <t>pracetice sql,  final exam</t>
+  </si>
+  <si>
+    <t>21 - 27 march</t>
+  </si>
+  <si>
+    <t>final exam module</t>
+  </si>
+  <si>
+    <t>thread, io, java 8</t>
+  </si>
+  <si>
+    <t>review practice, design software rule, design pattern, java generic</t>
+  </si>
+  <si>
+    <t>introduce java, 4 feature of java, package diagram</t>
+  </si>
+  <si>
+    <t>practice</t>
+  </si>
+  <si>
+    <t>java sql introduce, jdbc concept, synctax</t>
+  </si>
+  <si>
+    <t>practice session, upload file</t>
+  </si>
+  <si>
+    <t>practice session cart, filter</t>
+  </si>
+  <si>
+    <t>practice jdbc</t>
+  </si>
+  <si>
+    <t>- client &amp; server introduce
+- servlet concept
+- jsp 10 implicit object</t>
+  </si>
+  <si>
+    <t>practice servlet, jsp</t>
+  </si>
+  <si>
+    <t>- structure web app
+- web xml config
+- jsp expression tag
+- filter &amp; session</t>
+  </si>
+  <si>
+    <t>learn korea lesson 1</t>
+  </si>
+  <si>
+    <t>learn korea country vocal</t>
+  </si>
+  <si>
+    <t>break</t>
+  </si>
+  <si>
+    <t>28 march - 3 april</t>
+  </si>
+  <si>
+    <t>review from wed to now</t>
+  </si>
+  <si>
+    <t>scope, session, cookie, jstl custom tag</t>
   </si>
 </sst>
 </file>
@@ -167,26 +232,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -470,208 +550,369 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E2:L1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="45" customWidth="1"/>
+    <col min="9" max="9" width="28.28515625" customWidth="1"/>
     <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="2"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E3" s="3"/>
-      <c r="F3" s="4" t="s">
+      <c r="E3" s="2"/>
+      <c r="F3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
     </row>
     <row r="5" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
     </row>
     <row r="6" spans="5:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="6" t="s">
+      <c r="G6" s="4"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
     </row>
     <row r="7" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E7" s="5"/>
-      <c r="F7" s="6" t="s">
+      <c r="E7" s="4"/>
+      <c r="F7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
     </row>
     <row r="8" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
     </row>
     <row r="9" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="7" t="s">
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
     </row>
     <row r="10" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E10" s="3"/>
-      <c r="F10" s="4" t="s">
+      <c r="E10" s="2"/>
+      <c r="F10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="5:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="E11" s="4" t="s">
+    <row r="11" spans="5:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="E11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="5:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="E12" s="4" t="s">
+      <c r="I11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12" s="3"/>
+      <c r="H12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-    </row>
-    <row r="13" spans="5:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="G13" s="6" t="s">
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="5:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="G13" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="I13" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" s="12"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E16" s="7"/>
+      <c r="F16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="5:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="E17" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+    </row>
+    <row r="18" spans="5:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="E18" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+    </row>
+    <row r="19" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="I22" s="12"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+    </row>
+    <row r="23" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E23" s="7"/>
+      <c r="F23" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L23" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="5:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="E24" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" s="7"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+    </row>
+    <row r="25" spans="5:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="E25" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
     </row>
     <row r="1048576" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F1048576" s="1" t="s">
@@ -679,10 +920,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H22:I22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update lastweek at 2022-05-01
</commit_message>
<xml_diff>
--- a/Learning Detail.xlsx
+++ b/Learning Detail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="67">
   <si>
     <t>mon</t>
   </si>
@@ -176,6 +176,60 @@
   </si>
   <si>
     <t>scope, session, cookie, jstl custom tag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-10  april </t>
+  </si>
+  <si>
+    <t>11-17 april</t>
+  </si>
+  <si>
+    <t>springboot, spring annotation, springboot structure, spring pattern, di</t>
+  </si>
+  <si>
+    <t>thymeleaf concept, thymeleaf syntax, thymeleaf tag</t>
+  </si>
+  <si>
+    <t>thymeleaf fragment, spring session, springboot upload file</t>
+  </si>
+  <si>
+    <t>pratice all day: Xây 2 trang quản trị và trang người dùng quản sản phẩm</t>
+  </si>
+  <si>
+    <t>spring jdbc, spring data jdbc</t>
+  </si>
+  <si>
+    <t>hibernate core, hibernate annotaion</t>
+  </si>
+  <si>
+    <t>practice with hibernate configuration by annotaion</t>
+  </si>
+  <si>
+    <t>spring data jpa, syntax</t>
+  </si>
+  <si>
+    <t>pratice all day: xây dựng trang đăng ký môn học cho sinh viên</t>
+  </si>
+  <si>
+    <t>spring restfull, syntax</t>
+  </si>
+  <si>
+    <t>practice all day: xây dựng trang quản lý sản phẩm</t>
+  </si>
+  <si>
+    <t>practice jpa join</t>
+  </si>
+  <si>
+    <t>graphql, syntax, concept</t>
+  </si>
+  <si>
+    <t>18-24 april</t>
+  </si>
+  <si>
+    <t>practice graphql</t>
+  </si>
+  <si>
+    <t>reactive, webflux repository</t>
   </si>
 </sst>
 </file>
@@ -205,7 +259,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -228,11 +282,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -266,6 +346,24 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -550,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E2:L1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,10 +948,23 @@
         <v>44</v>
       </c>
     </row>
+    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>30</v>
+      </c>
+      <c r="I21">
+        <v>31</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+    </row>
     <row r="22" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
+      <c r="G22" s="6">
+        <v>29</v>
+      </c>
       <c r="H22" s="12" t="s">
         <v>46</v>
       </c>
@@ -886,17 +997,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="5:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:12" ht="75" x14ac:dyDescent="0.25">
       <c r="E24" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G24" s="7"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="7"/>
+      <c r="G24" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>54</v>
+      </c>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
     </row>
@@ -907,12 +1026,234 @@
       <c r="F25" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
+      <c r="G25" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J25" s="14"/>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
+    </row>
+    <row r="29" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I29" s="12"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+    </row>
+    <row r="30" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E30" s="7"/>
+      <c r="F30" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J30" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K30" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L30" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="5:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="E31" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H31" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="J31" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+    </row>
+    <row r="32" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E32" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H32" s="16"/>
+      <c r="I32" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J32" s="14"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+    </row>
+    <row r="36" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="I36" s="12"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+    </row>
+    <row r="37" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E37" s="7"/>
+      <c r="F37" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K37" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L37" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="5:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="E38" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H38" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="I38" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="J38" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+    </row>
+    <row r="39" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E39" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39" s="14"/>
+      <c r="G39" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+    </row>
+    <row r="44" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="I44" s="12"/>
+      <c r="J44" s="6"/>
+      <c r="K44" s="6"/>
+      <c r="L44" s="6"/>
+    </row>
+    <row r="45" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E45" s="7"/>
+      <c r="F45" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H45" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I45" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J45" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K45" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L45" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="5:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="E46" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="7"/>
+    </row>
+    <row r="47" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E47" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="18"/>
+      <c r="G47" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
     </row>
     <row r="1048576" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F1048576" s="1" t="s">
@@ -920,11 +1261,21 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="14">
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="J31:J32"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="I38:I39"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H29:I29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>